<commit_message>
Up to Table 6 autofilled
</commit_message>
<xml_diff>
--- a/design1/c998.xlsx
+++ b/design1/c998.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20378"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4355891\Documents\GitHub\MECH2100-Launchpad\main\Ass2\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MECH2100-A2\design1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7E866F-2219-4AF9-B262-1BEC4D3B50C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8819265-0FAD-4DDA-99F6-0B940868F296}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1830" yWindow="1830" windowWidth="17280" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -915,33 +915,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D42" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" customWidth="1"/>
-    <col min="21" max="21" width="63.140625" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" customWidth="1"/>
-    <col min="23" max="23" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.15625" customWidth="1"/>
+    <col min="2" max="2" width="4.68359375" customWidth="1"/>
+    <col min="3" max="3" width="16.15625" customWidth="1"/>
+    <col min="4" max="4" width="10.41796875" customWidth="1"/>
+    <col min="5" max="5" width="47.83984375" customWidth="1"/>
+    <col min="6" max="6" width="19.26171875" customWidth="1"/>
+    <col min="7" max="7" width="8.83984375" customWidth="1"/>
+    <col min="8" max="8" width="11.26171875" customWidth="1"/>
+    <col min="9" max="9" width="8.68359375" customWidth="1"/>
+    <col min="10" max="10" width="10.15625" customWidth="1"/>
+    <col min="11" max="11" width="8.68359375" customWidth="1"/>
+    <col min="13" max="13" width="10.83984375" customWidth="1"/>
+    <col min="14" max="14" width="8.68359375" customWidth="1"/>
+    <col min="19" max="19" width="9.15625" customWidth="1"/>
+    <col min="20" max="20" width="11.26171875" customWidth="1"/>
+    <col min="21" max="21" width="63.15625" customWidth="1"/>
+    <col min="22" max="22" width="9.15625" customWidth="1"/>
+    <col min="23" max="23" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" ht="25.8" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>129</v>
       </c>
@@ -950,13 +950,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -969,7 +969,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
         <v>4</v>
@@ -978,7 +978,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
         <v>5</v>
@@ -987,7 +987,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
@@ -998,7 +998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" s="2" t="s">
         <v>28</v>
       </c>
@@ -1129,7 +1129,7 @@
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="S17" s="2"/>
@@ -1138,7 +1138,7 @@
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
     </row>
-    <row r="18" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1155,7 +1155,7 @@
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" s="2" t="s">
         <v>32</v>
       </c>
@@ -1184,7 +1184,7 @@
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" s="2" t="s">
         <v>37</v>
       </c>
@@ -1236,7 +1236,7 @@
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" s="2" t="s">
         <v>38</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" s="2" t="s">
         <v>39</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="2" t="s">
         <v>42</v>
       </c>
@@ -1324,7 +1324,7 @@
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2">
         <v>5</v>
       </c>
@@ -1363,14 +1363,14 @@
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1386,7 +1386,7 @@
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" s="2" t="s">
         <v>49</v>
       </c>
@@ -1405,7 +1405,7 @@
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C29" s="2" t="s">
         <v>52</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" s="2" t="s">
         <v>55</v>
       </c>
@@ -1443,7 +1443,7 @@
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C31" s="2" t="s">
         <v>58</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="2" t="s">
         <v>60</v>
       </c>
@@ -1478,7 +1478,7 @@
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C33" s="2" t="s">
         <v>62</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="2" t="s">
         <v>64</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C35" s="2" t="s">
         <v>66</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2">
         <v>3</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2">
         <v>3</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2">
         <v>5</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>1807.6631706464509</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2">
         <v>10</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2">
         <v>10</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2">
         <v>10</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2">
         <v>10</v>
       </c>
@@ -1662,15 +1662,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C54" s="2" t="s">
         <v>6</v>
       </c>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C55" s="2" t="s">
         <v>32</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C56" s="2" t="s">
         <v>36</v>
       </c>
@@ -1706,7 +1706,7 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C57" s="2" t="s">
         <v>37</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C58" s="2" t="s">
         <v>38</v>
       </c>
@@ -1730,7 +1730,7 @@
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2">
         <v>3</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2">
         <v>3</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2">
         <v>3</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2">
         <v>3</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2">
         <v>3</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2">
         <v>3</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="2">
         <v>3</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2">
         <v>3</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="2">
         <v>3</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2">
         <v>3</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2">
         <v>3</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="2">
         <v>3</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="2">
         <v>3</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C73" s="2" t="s">
         <v>6</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C74" s="2" t="s">
         <v>32</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C75" s="2" t="s">
         <v>36</v>
       </c>
@@ -2103,7 +2103,7 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C76" s="2" t="s">
         <v>37</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C77" s="2" t="s">
         <v>38</v>
       </c>
@@ -2127,7 +2127,7 @@
       <c r="G77" s="10"/>
       <c r="H77" s="10"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="2">
         <v>10</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>-66671.96731057069</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="2">
         <v>10</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="2">
         <v>10</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>66671.96731057069</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="2">
         <v>10</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C91" s="2" t="s">
         <v>6</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C92" s="2" t="s">
         <v>32</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C93" s="2" t="s">
         <v>36</v>
       </c>
@@ -2260,7 +2260,7 @@
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C94" s="2" t="s">
         <v>37</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C95" s="2" t="s">
         <v>38</v>
       </c>
@@ -2284,7 +2284,7 @@
       <c r="G95" s="10"/>
       <c r="H95" s="10"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="2">
         <v>5</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>10.60454532231214</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="2">
         <v>5</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>-18.63</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="2">
         <v>5</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="2">
         <v>5</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>18.63</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C104" s="2" t="s">
         <v>6</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="2">
         <v>5</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="2">
         <v>5</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="2">
         <v>5</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="2">
         <v>5</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C118" s="2" t="s">
         <v>6</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C119" s="2" t="s">
         <v>32</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C120" s="2" t="s">
         <v>36</v>
       </c>
@@ -2478,7 +2478,7 @@
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C121" s="2" t="s">
         <v>37</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C122" s="2" t="s">
         <v>38</v>
       </c>
@@ -2502,7 +2502,7 @@
       <c r="G122" s="10"/>
       <c r="H122" s="10"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="2">
         <v>10</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>15.90681798346821</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="2">
         <v>10</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>-22.356000000000002</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="2">
         <v>10</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="2">
         <v>10</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>22.356000000000002</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="C136" s="2" t="s">
         <v>6</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="2">
         <v>50</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="2">
         <v>50</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>33.299837208616403</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="2">
         <v>50</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>33.04162258102059</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -2676,7 +2676,7 @@
       <c r="N141" s="2"/>
       <c r="O141" s="2"/>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -2693,7 +2693,7 @@
       <c r="N142" s="2"/>
       <c r="O142" s="2"/>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -2710,7 +2710,7 @@
       <c r="N143" s="2"/>
       <c r="O143" s="2"/>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -2727,7 +2727,7 @@
       <c r="N144" s="2"/>
       <c r="O144" s="2"/>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -2744,7 +2744,7 @@
       <c r="N145" s="2"/>
       <c r="O145" s="2"/>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -2761,7 +2761,7 @@
       <c r="N146" s="2"/>
       <c r="O146" s="2"/>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -2778,7 +2778,7 @@
       <c r="N147" s="2"/>
       <c r="O147" s="2"/>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -2795,7 +2795,7 @@
       <c r="N148" s="2"/>
       <c r="O148" s="2"/>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -2812,7 +2812,7 @@
       <c r="N149" s="2"/>
       <c r="O149" s="2"/>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -2829,7 +2829,7 @@
       <c r="N150" s="2"/>
       <c r="O150" s="2"/>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -2846,7 +2846,7 @@
       <c r="N151" s="2"/>
       <c r="O151" s="2"/>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -2863,7 +2863,7 @@
       <c r="N152" s="2"/>
       <c r="O152" s="2"/>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -2880,7 +2880,7 @@
       <c r="N153" s="2"/>
       <c r="O153" s="2"/>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -2897,7 +2897,7 @@
       <c r="N154" s="2"/>
       <c r="O154" s="2"/>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -2914,7 +2914,7 @@
       <c r="N155" s="2"/>
       <c r="O155" s="2"/>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -2931,7 +2931,7 @@
       <c r="N156" s="2"/>
       <c r="O156" s="2"/>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -2948,7 +2948,7 @@
       <c r="N157" s="2"/>
       <c r="O157" s="2"/>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>

</xml_diff>

<commit_message>
Fatigue life computed correctly
</commit_message>
<xml_diff>
--- a/design1/c998.xlsx
+++ b/design1/c998.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MECH2100-A2\design1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Projects\MECH2100-A2\design1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16ADF99-F73B-43B5-BD97-54BDFD21A835}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7920521-A274-4D81-8E30-0253E7238320}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="5970" windowWidth="17280" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40860" yWindow="2760" windowWidth="17130" windowHeight="6315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -915,33 +915,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="G154" workbookViewId="0">
+      <selection activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.15625" customWidth="1"/>
-    <col min="2" max="2" width="4.68359375" customWidth="1"/>
-    <col min="3" max="3" width="16.15625" customWidth="1"/>
-    <col min="4" max="4" width="10.41796875" customWidth="1"/>
-    <col min="5" max="5" width="47.83984375" customWidth="1"/>
-    <col min="6" max="6" width="19.26171875" customWidth="1"/>
-    <col min="7" max="7" width="8.83984375" customWidth="1"/>
-    <col min="8" max="8" width="11.26171875" customWidth="1"/>
-    <col min="9" max="9" width="8.68359375" customWidth="1"/>
-    <col min="10" max="10" width="10.15625" customWidth="1"/>
-    <col min="11" max="11" width="8.68359375" customWidth="1"/>
-    <col min="13" max="13" width="10.83984375" customWidth="1"/>
-    <col min="14" max="14" width="8.68359375" customWidth="1"/>
-    <col min="19" max="19" width="9.15625" customWidth="1"/>
-    <col min="20" max="20" width="11.26171875" customWidth="1"/>
-    <col min="21" max="21" width="63.15625" customWidth="1"/>
-    <col min="22" max="22" width="9.15625" customWidth="1"/>
-    <col min="23" max="23" width="8.68359375" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="47.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" customWidth="1"/>
+    <col min="19" max="19" width="9.109375" customWidth="1"/>
+    <col min="20" max="20" width="11.21875" customWidth="1"/>
+    <col min="21" max="21" width="63.109375" customWidth="1"/>
+    <col min="22" max="22" width="9.109375" customWidth="1"/>
+    <col min="23" max="23" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="25.8" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:23" ht="25.2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>129</v>
       </c>
@@ -950,13 +950,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -969,7 +969,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
         <v>4</v>
@@ -978,7 +978,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
         <v>5</v>
@@ -987,7 +987,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
@@ -998,7 +998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
         <v>28</v>
       </c>
@@ -1129,7 +1129,7 @@
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="S17" s="2"/>
@@ -1138,7 +1138,7 @@
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
     </row>
-    <row r="18" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1155,7 +1155,7 @@
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C19" s="2" t="s">
         <v>32</v>
       </c>
@@ -1184,7 +1184,7 @@
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="s">
         <v>37</v>
       </c>
@@ -1236,7 +1236,7 @@
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C22" s="2" t="s">
         <v>38</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C23" s="2" t="s">
         <v>39</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C24" s="2" t="s">
         <v>42</v>
       </c>
@@ -1324,7 +1324,7 @@
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>5</v>
       </c>
@@ -1363,14 +1363,14 @@
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1386,7 +1386,7 @@
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C28" s="2" t="s">
         <v>49</v>
       </c>
@@ -1405,7 +1405,7 @@
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C29" s="2" t="s">
         <v>52</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C30" s="2" t="s">
         <v>55</v>
       </c>
@@ -1443,7 +1443,7 @@
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C31" s="2" t="s">
         <v>58</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C32" s="2" t="s">
         <v>60</v>
       </c>
@@ -1478,7 +1478,7 @@
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C33" s="2" t="s">
         <v>62</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C34" s="2" t="s">
         <v>64</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C35" s="2" t="s">
         <v>66</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>3</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>3</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>5</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>1807.6631706464509</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>10</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>10</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>10</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>10</v>
       </c>
@@ -1662,15 +1662,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C54" s="2" t="s">
         <v>6</v>
       </c>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C55" s="2" t="s">
         <v>32</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C56" s="2" t="s">
         <v>36</v>
       </c>
@@ -1706,7 +1706,7 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C57" s="2" t="s">
         <v>37</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C58" s="2" t="s">
         <v>38</v>
       </c>
@@ -1730,7 +1730,7 @@
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>3</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>3</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>3</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>3</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>3</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>3</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>3</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>3</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>3</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>3</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>3</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>3</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>3</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C73" s="2" t="s">
         <v>6</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C74" s="2" t="s">
         <v>32</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C75" s="2" t="s">
         <v>36</v>
       </c>
@@ -2103,7 +2103,7 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C76" s="2" t="s">
         <v>37</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C77" s="2" t="s">
         <v>38</v>
       </c>
@@ -2127,7 +2127,7 @@
       <c r="G77" s="10"/>
       <c r="H77" s="10"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>10</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>-66671.96731057069</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>10</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>10</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>66671.96731057069</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>10</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C91" s="2" t="s">
         <v>6</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C92" s="2" t="s">
         <v>32</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C93" s="2" t="s">
         <v>36</v>
       </c>
@@ -2260,7 +2260,7 @@
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C94" s="2" t="s">
         <v>37</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C95" s="2" t="s">
         <v>38</v>
       </c>
@@ -2284,7 +2284,7 @@
       <c r="G95" s="10"/>
       <c r="H95" s="10"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>5</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>10.60454532231214</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>5</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>-18.63</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>5</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>5</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>18.63</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C104" s="2" t="s">
         <v>6</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>5</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>5</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>5</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>5</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C118" s="2" t="s">
         <v>6</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C119" s="2" t="s">
         <v>32</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C120" s="2" t="s">
         <v>36</v>
       </c>
@@ -2478,7 +2478,7 @@
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C121" s="2" t="s">
         <v>37</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C122" s="2" t="s">
         <v>38</v>
       </c>
@@ -2502,7 +2502,7 @@
       <c r="G122" s="10"/>
       <c r="H122" s="10"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>10</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>15.90681798346821</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>10</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>-22.356000000000002</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>10</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>10</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>22.356000000000002</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C136" s="2" t="s">
         <v>6</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <v>50</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>50</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>33.299837208616403</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
         <v>50</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>33.04162258102059</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -2676,7 +2676,7 @@
       <c r="N141" s="2"/>
       <c r="O141" s="2"/>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -2693,7 +2693,7 @@
       <c r="N142" s="2"/>
       <c r="O142" s="2"/>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -2710,7 +2710,7 @@
       <c r="N143" s="2"/>
       <c r="O143" s="2"/>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -2727,7 +2727,7 @@
       <c r="N144" s="2"/>
       <c r="O144" s="2"/>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -2744,7 +2744,7 @@
       <c r="N145" s="2"/>
       <c r="O145" s="2"/>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -2761,7 +2761,7 @@
       <c r="N146" s="2"/>
       <c r="O146" s="2"/>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -2778,7 +2778,7 @@
       <c r="N147" s="2"/>
       <c r="O147" s="2"/>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -2795,7 +2795,7 @@
       <c r="N148" s="2"/>
       <c r="O148" s="2"/>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -2812,7 +2812,7 @@
       <c r="N149" s="2"/>
       <c r="O149" s="2"/>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -2829,7 +2829,7 @@
       <c r="N150" s="2"/>
       <c r="O150" s="2"/>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -2846,7 +2846,7 @@
       <c r="N151" s="2"/>
       <c r="O151" s="2"/>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -2863,7 +2863,7 @@
       <c r="N152" s="2"/>
       <c r="O152" s="2"/>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -2880,7 +2880,7 @@
       <c r="N153" s="2"/>
       <c r="O153" s="2"/>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -2897,7 +2897,7 @@
       <c r="N154" s="2"/>
       <c r="O154" s="2"/>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -2914,7 +2914,7 @@
       <c r="N155" s="2"/>
       <c r="O155" s="2"/>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -2931,7 +2931,7 @@
       <c r="N156" s="2"/>
       <c r="O156" s="2"/>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -2948,7 +2948,7 @@
       <c r="N157" s="2"/>
       <c r="O157" s="2"/>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>

</xml_diff>